<commit_message>
Subida de evidencias y estructura de git solicitado
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentación/Plantilla Historias Usuario.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentación/Plantilla Historias Usuario.xlsx
@@ -5,20 +5,19 @@
   <sheets>
     <sheet state="visible" name="Historias de Usuario" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Instructivo" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="ejemplo_historia" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="qOLxCcx5eJx5IdxWjTPrhYIwB/r8mOfDtJ81ordUbFw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="Kk+80PmVWl63XDTiLtUTGFfAC/2rxX5mKLx517m3bUs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="195">
   <si>
     <t>Desarrollo ágil: Historias de usuario y criterios de aceptación</t>
   </si>
@@ -56,403 +55,511 @@
     <t>Resultado / Comportamiento esperado</t>
   </si>
   <si>
-    <t>E01-HU1</t>
+    <t>HU1</t>
   </si>
   <si>
-    <t>Jugador</t>
+    <t>Usuario</t>
   </si>
   <si>
-    <t>Registro de usuarios</t>
+    <t>Registro de usuario</t>
   </si>
   <si>
-    <t>Para que pueda crear una cuenta y acceder a la plataforma</t>
+    <t>Acceder a la plataforma</t>
   </si>
   <si>
-    <t>Campos válidos</t>
+    <t>Registro exitoso</t>
   </si>
   <si>
-    <t>El usuario está en la página de registro</t>
+    <t>El usuario abre la página de registro.</t>
   </si>
   <si>
-    <t>El usuario ingresa datos válidos</t>
+    <t>Completa el formulario con datos válidos y lo envía.</t>
   </si>
   <si>
-    <t>El sistema registra al usuario y muestra un mensaje de confirmación.</t>
+    <t>El sistema crea una cuenta y muestra un mensaje de confirmación.</t>
   </si>
   <si>
-    <t>Campos inválidos</t>
+    <t>HU2</t>
   </si>
   <si>
-    <t>El usuario ingresa datos inválidos</t>
+    <t>Inicio de sesión</t>
   </si>
   <si>
-    <t>El sistema muestra un mensaje de error indicando qué campos son incorrectos.</t>
+    <t>Acceder a funcionalidades personalizadas</t>
   </si>
   <si>
-    <t>Confirmación de correo</t>
+    <t>Autenticación correcta</t>
   </si>
   <si>
-    <t>El usuario completa el registro</t>
+    <t>El usuario abre la página de inicio de sesión.</t>
   </si>
   <si>
-    <t>El sistema envía un correo de verificación</t>
+    <t>Ingresa credenciales correctas y las envía.</t>
   </si>
   <si>
-    <t>El usuario recibe un correo electrónico para confirmar su cuenta.</t>
+    <t>El sistema verifica los datos y permite el acceso.</t>
   </si>
   <si>
-    <t>E02-HU2</t>
+    <t>HU3</t>
+  </si>
+  <si>
+    <t>Recuperación de contraseña</t>
+  </si>
+  <si>
+    <t>Recuperar acceso a la cuenta</t>
+  </si>
+  <si>
+    <t>Contraseña restablecida</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Olvidé mi contraseña".</t>
+  </si>
+  <si>
+    <t>Proporciona el correo asociado a la cuenta.</t>
+  </si>
+  <si>
+    <t>El sistema envía un correo con instrucciones para restablecer la contraseña.</t>
+  </si>
+  <si>
+    <t>HU4</t>
+  </si>
+  <si>
+    <t>Actualización de perfil</t>
+  </si>
+  <si>
+    <t>Mantener su información actualizada</t>
+  </si>
+  <si>
+    <t>Perfil actualizado</t>
+  </si>
+  <si>
+    <t>El usuario abre la página de perfil.</t>
+  </si>
+  <si>
+    <t>Modifica los datos personales y los guarda.</t>
+  </si>
+  <si>
+    <t>El sistema guarda los cambios y muestra un mensaje de éxito.</t>
+  </si>
+  <si>
+    <t>HU5</t>
+  </si>
+  <si>
+    <t>Creación de partidos</t>
+  </si>
+  <si>
+    <t>Organizar eventos deportivos</t>
+  </si>
+  <si>
+    <t>Partido creado</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Crear partido".</t>
+  </si>
+  <si>
+    <t>Ingresa detalles del partido y los confirma.</t>
+  </si>
+  <si>
+    <t>El sistema registra el partido y lo muestra en la lista de partidos disponibles.</t>
+  </si>
+  <si>
+    <t>HU6</t>
+  </si>
+  <si>
+    <t>Buscar partidos</t>
+  </si>
+  <si>
+    <t>Unirse a eventos deportivos</t>
+  </si>
+  <si>
+    <t>Partidos mostrados</t>
+  </si>
+  <si>
+    <t>El usuario abre la sección de búsqueda de partidos.</t>
+  </si>
+  <si>
+    <t>Proporciona filtros de ubicación y horario.</t>
+  </si>
+  <si>
+    <t>El sistema muestra partidos que coincidan con los filtros.</t>
+  </si>
+  <si>
+    <t>HU7</t>
+  </si>
+  <si>
+    <t>Reservar cancha</t>
+  </si>
+  <si>
+    <t>Asegurar espacio para jugar</t>
+  </si>
+  <si>
+    <t>Reserva completada</t>
+  </si>
+  <si>
+    <t>El usuario selecciona una cancha disponible.</t>
+  </si>
+  <si>
+    <t>Ingresa detalles de la reserva y los confirma.</t>
+  </si>
+  <si>
+    <t>El sistema registra la reserva y envía una notificación de confirmación.</t>
+  </si>
+  <si>
+    <t>HU8</t>
+  </si>
+  <si>
+    <t>Enviar notificaciones</t>
+  </si>
+  <si>
+    <t>Informar a los jugadores sobre cambios o actualizaciones</t>
+  </si>
+  <si>
+    <t>Notificación enviada</t>
+  </si>
+  <si>
+    <t>El sistema detecta un cambio en el partido o reserva.</t>
+  </si>
+  <si>
+    <t>Genera y envía una notificación al usuario afectado.</t>
+  </si>
+  <si>
+    <t>Los jugadores reciben la notificación en tiempo real.</t>
+  </si>
+  <si>
+    <t>HU9</t>
+  </si>
+  <si>
+    <t>Realizar pagos</t>
+  </si>
+  <si>
+    <t>Completar transacciones de reservas</t>
+  </si>
+  <si>
+    <t>Pago exitoso</t>
+  </si>
+  <si>
+    <t>El usuario selecciona un método de pago.</t>
+  </si>
+  <si>
+    <t>Proporciona los datos requeridos y confirma el pago.</t>
+  </si>
+  <si>
+    <t>El sistema procesa el pago y muestra un comprobante de transacción.</t>
+  </si>
+  <si>
+    <t>HU10</t>
+  </si>
+  <si>
+    <t>Consultar historial de pagos</t>
+  </si>
+  <si>
+    <t>Mantener control sobre transacciones</t>
+  </si>
+  <si>
+    <t>Historial mostrado</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Historial de pagos".</t>
+  </si>
+  <si>
+    <t>El sistema recupera y muestra todas las transacciones realizadas.</t>
+  </si>
+  <si>
+    <t>Los datos de las transacciones se presentan con detalle y opciones de descarga.</t>
+  </si>
+  <si>
+    <t>HU11</t>
+  </si>
+  <si>
+    <t>Visualizar estadísticas</t>
+  </si>
+  <si>
+    <t>Evaluar rendimiento personal</t>
+  </si>
+  <si>
+    <t>Estadísticas mostradas</t>
+  </si>
+  <si>
+    <t>El usuario abre la sección de estadísticas.</t>
+  </si>
+  <si>
+    <t>Selecciona el tipo de estadísticas a visualizar.</t>
+  </si>
+  <si>
+    <t>El sistema muestra gráficos y datos relevantes del rendimiento del usuario.</t>
+  </si>
+  <si>
+    <t>HU12</t>
+  </si>
+  <si>
+    <t>Comparar rendimiento con otros jugadores</t>
+  </si>
+  <si>
+    <t>Evaluar nivel competitivo</t>
+  </si>
+  <si>
+    <t>Comparación exitosa</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Comparar rendimiento".</t>
+  </si>
+  <si>
+    <t>El sistema solicita el jugador a comparar.</t>
+  </si>
+  <si>
+    <t>Se presentan gráficos comparativos y datos clave.</t>
+  </si>
+  <si>
+    <t>HU13</t>
+  </si>
+  <si>
+    <t>Consultar historial de partidos</t>
+  </si>
+  <si>
+    <t>Revisar encuentros anteriores</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Historial de partidos".</t>
+  </si>
+  <si>
+    <t>El sistema recupera la lista de partidos jugados.</t>
+  </si>
+  <si>
+    <t>Los partidos se muestran con detalles como fecha, lugar y resultado.</t>
+  </si>
+  <si>
+    <t>HU14</t>
+  </si>
+  <si>
+    <t>Visualizar logros</t>
+  </si>
+  <si>
+    <t>Ver lista de logros alcanzados y pendientes</t>
+  </si>
+  <si>
+    <t>Logros visibles</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la sección de logros en el perfil.</t>
+  </si>
+  <si>
+    <t>Se cargan todos los logros alcanzados y los disponibles.</t>
+  </si>
+  <si>
+    <t>El sistema permite visualizar los logros con opciones para compartir.</t>
+  </si>
+  <si>
+    <t>HU15</t>
+  </si>
+  <si>
+    <t>Compartir logros</t>
+  </si>
+  <si>
+    <t>Compartir logros con otros jugadores</t>
+  </si>
+  <si>
+    <t>Logros compartidos</t>
+  </si>
+  <si>
+    <t>El usuario selecciona un logro alcanzado y la opción de compartir.</t>
+  </si>
+  <si>
+    <t>El sistema genera un enlace o envía notificaciones del logro compartido.</t>
+  </si>
+  <si>
+    <t>Los destinatarios reciben el logro compartido.</t>
+  </si>
+  <si>
+    <t>HU16</t>
+  </si>
+  <si>
+    <t>Consultar información de FlashMatch</t>
+  </si>
+  <si>
+    <t>Conocer características de la plataforma</t>
+  </si>
+  <si>
+    <t>Información presentada</t>
+  </si>
+  <si>
+    <t>El usuario accede a la página principal de la aplicación.</t>
+  </si>
+  <si>
+    <t>Navega por las secciones de misión, visión y funcionalidades.</t>
+  </si>
+  <si>
+    <t>La plataforma presenta información clara y accesible.</t>
+  </si>
+  <si>
+    <t>HU17</t>
+  </si>
+  <si>
+    <t>Crear perfil de equipo</t>
+  </si>
+  <si>
+    <t>Organizar equipos para partidos</t>
+  </si>
+  <si>
+    <t>Perfil de equipo creado</t>
+  </si>
+  <si>
+    <t>El usuario selecciona la opción "Crear equipo".</t>
+  </si>
+  <si>
+    <t>Ingresa los datos del equipo y los confirma.</t>
+  </si>
+  <si>
+    <t>El sistema registra el equipo y lo asocia con el perfil del usuario.</t>
+  </si>
+  <si>
+    <t>HU18</t>
+  </si>
+  <si>
+    <t>Gestionar roles dentro del equipo</t>
+  </si>
+  <si>
+    <t>Asignar roles a los miembros del equipo</t>
+  </si>
+  <si>
+    <t>Roles asignados correctamente</t>
+  </si>
+  <si>
+    <t>El administrador del equipo selecciona la opción "Gestionar roles".</t>
+  </si>
+  <si>
+    <t>Asigna roles como capitán, jugador o suplente.</t>
+  </si>
+  <si>
+    <t>El sistema actualiza la lista de roles para cada miembro del equipo.</t>
+  </si>
+  <si>
+    <t>HU19</t>
   </si>
   <si>
     <t>Administrador</t>
   </si>
   <si>
-    <t>Gestión de reservas de canchas</t>
+    <t>Aprobar solicitudes de nuevos equipos</t>
   </si>
   <si>
-    <t>Para gestionar y confirmar reservas de canchas</t>
+    <t>Mantener un registro de equipos registrados</t>
   </si>
   <si>
-    <t>Reserva creada y confirmada</t>
+    <t>Equipo aprobado</t>
   </si>
   <si>
-    <t>El administrador está en la interfaz de reservas</t>
+    <t>El administrador recibe la solicitud de un equipo para registrarse en el sistema.</t>
   </si>
   <si>
-    <t>El administrador crea una nueva reserva</t>
+    <t>Revisa los datos del equipo y selecciona "Aprobar".</t>
   </si>
   <si>
-    <t>El sistema guarda la reserva y envía notificaciones a los usuarios y al administrador.</t>
+    <t>El sistema actualiza el estado del equipo como "Activo" en la base de datos.</t>
   </si>
   <si>
-    <t>Cancelación de reserva</t>
+    <t>HU20</t>
   </si>
   <si>
-    <t>El administrador visualiza las reservas</t>
+    <t>Enviar invitaciones a jugadores</t>
   </si>
   <si>
-    <t>El administrador cancela una reserva</t>
+    <t>Completar el equipo para un partido</t>
   </si>
   <si>
-    <t>El sistema actualiza el estado de la reserva y notifica a los usuarios afectados.</t>
+    <t>Invitaciones enviadas</t>
   </si>
   <si>
-    <t>Visualización de reservas disponibles</t>
+    <t>El usuario selecciona un partido y la opción "Invitar jugadores".</t>
   </si>
   <si>
-    <t>El administrador accede a la lista de reservas</t>
+    <t>Ingresa los datos del jugador o selecciona de su lista de contactos.</t>
   </si>
   <si>
-    <t>El administrador busca canchas disponibles</t>
+    <t>El sistema envía la invitación y registra el estado como "Pendiente de respuesta".</t>
   </si>
   <si>
-    <t>El sistema muestra una lista de canchas disponibles para reservar.</t>
+    <t>HU21</t>
   </si>
   <si>
-    <t>E03-HU3</t>
+    <t>Consultar notificaciones</t>
   </si>
   <si>
-    <t>Búsqueda de partidos disponibles</t>
+    <t>Revisar actualizaciones sobre partidos, reservas y pagos</t>
   </si>
   <si>
-    <t>Para encontrar partidos en mi área en los que pueda participar</t>
+    <t>Notificaciones mostradas</t>
   </si>
   <si>
-    <t>Visualización de partidos disponibles</t>
+    <t>El usuario abre la sección de notificaciones en la app.</t>
   </si>
   <si>
-    <t>El jugador selecciona buscar partidos</t>
+    <t>El sistema carga todas las notificaciones recientes.</t>
   </si>
   <si>
-    <t>El jugador ingresa su ubicación</t>
+    <t>El usuario puede interactuar con las notificaciones, como aceptar o rechazar eventos.</t>
   </si>
   <si>
-    <t>El sistema muestra partidos disponibles según la ubicación del jugador.</t>
+    <t>HU22</t>
   </si>
   <si>
-    <t>Filtros de búsqueda</t>
+    <t>Configurar preferencias de notificaciones</t>
   </si>
   <si>
-    <t>El jugador está en la página de búsqueda</t>
+    <t>Personalizar alertas y actualizaciones</t>
   </si>
   <si>
-    <t>El jugador aplica filtros</t>
+    <t>Preferencias guardadas</t>
   </si>
   <si>
-    <t>El sistema muestra partidos filtrados según los criterios seleccionados.</t>
+    <t>El usuario selecciona la opción "Configuración de notificaciones".</t>
   </si>
   <si>
-    <t>Unirse a un partido</t>
+    <t>Activa o desactiva tipos específicos de alertas.</t>
   </si>
   <si>
-    <t>El jugador visualiza un partido</t>
+    <t>El sistema guarda las preferencias y actualiza el envío de notificaciones.</t>
   </si>
   <si>
-    <t>El jugador hace clic en "Unirse"</t>
+    <t>HU23</t>
   </si>
   <si>
-    <t>El sistema agrega al jugador al partido y envía notificación a los participantes.</t>
+    <t>Descargar comprobantes de pagos</t>
   </si>
   <si>
-    <t>E04-HU4</t>
+    <t>Mantener un registro físico o digital de transacciones</t>
   </si>
   <si>
-    <t>Visualización de estadísticas</t>
+    <t>Comprobante descargado</t>
   </si>
   <si>
-    <t>Para ver estadísticas de uso y rendimiento de las canchas</t>
+    <t>El usuario selecciona una transacción en el historial de pagos.</t>
   </si>
   <si>
-    <t>Estadísticas de reservas</t>
+    <t>Pulsa la opción "Descargar comprobante".</t>
   </si>
   <si>
-    <t>El administrador está en la sección de estadísticas</t>
+    <t>El sistema genera un archivo PDF del comprobante y lo descarga.</t>
   </si>
   <si>
-    <t>El administrador solicita ver estadísticas</t>
+    <t>HU24</t>
   </si>
   <si>
-    <t>El sistema muestra un informe detallado con estadísticas de uso de canchas.</t>
+    <t>Completar formulario de contacto</t>
   </si>
   <si>
-    <t>Comparación de canchas</t>
+    <t>Enviar consultas o comentarios al equipo de soporte</t>
   </si>
   <si>
-    <t>El administrador quiere comparar canchas</t>
+    <t>Mensaje enviado</t>
   </si>
   <si>
-    <t>El administrador selecciona dos canchas</t>
+    <t>El usuario abre la sección "Contacto" en la página de presentación.</t>
   </si>
   <si>
-    <t>El sistema presenta un gráfico comparativo del uso de las canchas seleccionadas.</t>
+    <t>Llena el formulario con sus datos y mensaje.</t>
   </si>
   <si>
-    <t>E05-HU5</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Notificaciones sobre partidos próximos</t>
-  </si>
-  <si>
-    <t>Para recibir alertas de partidos próximos</t>
-  </si>
-  <si>
-    <t>Notificación recibida a tiempo</t>
-  </si>
-  <si>
-    <t>Un partido está próximo</t>
-  </si>
-  <si>
-    <t>El sistema envía una notificación al usuario</t>
-  </si>
-  <si>
-    <t>El usuario recibe una notificación con los detalles del partido (fecha, hora, lugar).</t>
-  </si>
-  <si>
-    <t>Notificación de cambio de horario</t>
-  </si>
-  <si>
-    <t>Un partido programado cambia de hora</t>
-  </si>
-  <si>
-    <t>El sistema actualiza la notificación</t>
-  </si>
-  <si>
-    <t>El usuario recibe una actualización sobre el cambio de horario del partido.</t>
-  </si>
-  <si>
-    <t>E06-HU6</t>
-  </si>
-  <si>
-    <t>Actualización de perfil</t>
-  </si>
-  <si>
-    <t>Para gestionar mi información personal</t>
-  </si>
-  <si>
-    <t>Actualización exitosa</t>
-  </si>
-  <si>
-    <t>El jugador está en la página de perfil</t>
-  </si>
-  <si>
-    <t>El jugador modifica su información y presiona "Actualizar".</t>
-  </si>
-  <si>
-    <t>El sistema actualiza la información y muestra un mensaje de éxito.</t>
-  </si>
-  <si>
-    <t>Datos inválidos</t>
-  </si>
-  <si>
-    <t>El jugador ingresa datos incorrectos</t>
-  </si>
-  <si>
-    <t>Presiona "Actualizar".</t>
-  </si>
-  <si>
-    <t>E07-HU7</t>
-  </si>
-  <si>
-    <t>Reportes de reservas y estadísticas</t>
-  </si>
-  <si>
-    <t>Para revisar la ocupación y utilización de las canchas</t>
-  </si>
-  <si>
-    <t>Informe de reservas</t>
-  </si>
-  <si>
-    <t>El administrador está en la sección de reportes</t>
-  </si>
-  <si>
-    <t>El administrador solicita ver un informe de reservas.</t>
-  </si>
-  <si>
-    <t>El sistema muestra el informe solicitado.</t>
-  </si>
-  <si>
-    <t>E08-HU8</t>
-  </si>
-  <si>
-    <t>Agregar direcciones</t>
-  </si>
-  <si>
-    <t>Para coordinar la ubicación de los partidos y reservas</t>
-  </si>
-  <si>
-    <t>Dirección añadida</t>
-  </si>
-  <si>
-    <t>El jugador ingresa una nueva dirección y presiona "Agregar".</t>
-  </si>
-  <si>
-    <t>El sistema guarda la dirección y muestra un mensaje de confirmación.</t>
-  </si>
-  <si>
-    <t>E09-HU9</t>
-  </si>
-  <si>
-    <t>Revisar estado de inscripción</t>
-  </si>
-  <si>
-    <t>Para asegurar que mi participación esté confirmada</t>
-  </si>
-  <si>
-    <t>Estado de inscripción</t>
-  </si>
-  <si>
-    <t>El jugador está en su perfil</t>
-  </si>
-  <si>
-    <t>El jugador revisa el estado de inscripción</t>
-  </si>
-  <si>
-    <t>El sistema muestra el estado actual de la inscripción.</t>
-  </si>
-  <si>
-    <t>E10-HU10</t>
-  </si>
-  <si>
-    <t>Visualización de informes de rendimiento</t>
-  </si>
-  <si>
-    <t>Para realizar ajustes en la organización de partidos</t>
-  </si>
-  <si>
-    <t>Informe detallado</t>
-  </si>
-  <si>
-    <t>El administrador solicita informes</t>
-  </si>
-  <si>
-    <t>El administrador selecciona el periodo de tiempo.</t>
-  </si>
-  <si>
-    <t>El sistema muestra el informe detallado de uso y rendimiento.</t>
-  </si>
-  <si>
-    <t>E11-HU11</t>
-  </si>
-  <si>
-    <t>Elección de sistema de pago</t>
-  </si>
-  <si>
-    <t>Para completar reservas y pagos asociados</t>
-  </si>
-  <si>
-    <t>Pago exitoso</t>
-  </si>
-  <si>
-    <t>El jugador está en la página de pago</t>
-  </si>
-  <si>
-    <t>El jugador selecciona un método de pago y completa la transacción.</t>
-  </si>
-  <si>
-    <t>El sistema confirma el pago y muestra un mensaje de éxito.</t>
-  </si>
-  <si>
-    <t>E12-HU12</t>
-  </si>
-  <si>
-    <t>Permisos de modificación en la plataforma</t>
-  </si>
-  <si>
-    <t>Para realizar ajustes en detalles de partidos y canchas</t>
-  </si>
-  <si>
-    <t>Permisos concedidos</t>
-  </si>
-  <si>
-    <t>El administrador accede a la configuración</t>
-  </si>
-  <si>
-    <t>El administrador solicita permisos adicionales.</t>
-  </si>
-  <si>
-    <t>El sistema otorga los permisos necesarios.</t>
-  </si>
-  <si>
-    <t>E13-HU13</t>
-  </si>
-  <si>
-    <t>Para realizar compras o arriendos</t>
-  </si>
-  <si>
-    <t>Selección de pago</t>
-  </si>
-  <si>
-    <t>El jugador está en la sección de pago</t>
-  </si>
-  <si>
-    <t>El jugador selecciona el sistema de pago deseado.</t>
-  </si>
-  <si>
-    <t>El sistema procesa la selección y muestra los detalles.</t>
-  </si>
-  <si>
-    <t>E14-HU14</t>
-  </si>
-  <si>
-    <t>Rellenar un formulario</t>
-  </si>
-  <si>
-    <t>Para inscribirme en un partido y gestionar mi participación</t>
-  </si>
-  <si>
-    <t>Formulario enviado</t>
-  </si>
-  <si>
-    <t>El usuario está en la página del formulario</t>
-  </si>
-  <si>
-    <t>El usuario completa el formulario y presiona "Enviar".</t>
-  </si>
-  <si>
-    <t>El sistema recibe el formulario y muestra un mensaje de confirmación.</t>
+    <t>El sistema envía el mensaje al equipo de soporte y muestra una confirmación.</t>
   </si>
   <si>
     <t>Historias de usuario y criterios de aceptación: Instructivo</t>
@@ -503,60 +610,12 @@
   <si>
     <t>Dado el contexto y la acción ejecutada por el usuario, la consecuencia es el comportamiento del sistema en esa situación.</t>
   </si>
-  <si>
-    <t>Historias de usuario y criterios de aceptación: Ejemplo</t>
-  </si>
-  <si>
-    <t>Historia de Usuario</t>
-  </si>
-  <si>
-    <t>H001</t>
-  </si>
-  <si>
-    <t>Como un cliente o ejecutivo de ventas</t>
-  </si>
-  <si>
-    <t>Necesito ver un listado de contratos y poder seleccionar alguno para ver sus servicios.</t>
-  </si>
-  <si>
-    <t>Con la finalidad de obtener información de los servicios adicionales contratados.</t>
-  </si>
-  <si>
-    <t>Contratos  con al menos un servicio.</t>
-  </si>
-  <si>
-    <t>En caso que un contrato tenga al menos un servicio asociado.</t>
-  </si>
-  <si>
-    <t>Cuando se despliegue el listado de contratos  a seleccionar.</t>
-  </si>
-  <si>
-    <t>A continuación del número del contrato, se mostrará el número de productos asociados.</t>
-  </si>
-  <si>
-    <t>Contrato sin servicios.</t>
-  </si>
-  <si>
-    <t>En caso que una contrato no tenga servicios asociados.</t>
-  </si>
-  <si>
-    <t>A continuación del número del contrato, se mostrará el siguiente texto "Sin servicios asociados".</t>
-  </si>
-  <si>
-    <t>Ordenamiento de los contratos</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>El sistema mostrará los contratos en orden de fecha de contrato.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -588,18 +647,12 @@
     <font/>
     <font>
       <b/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="24.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,26 +671,8 @@
         <bgColor rgb="FF1F497D"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFBFBFBF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF95B3D7"/>
-        <bgColor rgb="FF95B3D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF953734"/>
-        <bgColor rgb="FF953734"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="7">
     <border/>
     <border>
       <left/>
@@ -688,62 +723,6 @@
       <bottom/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -757,167 +736,17 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -926,81 +755,14 @@
     <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="20" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1014,10 +776,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1227,7 +985,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="1.43"/>
     <col customWidth="1" min="2" max="2" width="13.71"/>
-    <col customWidth="1" min="3" max="3" width="14.43"/>
     <col customWidth="1" min="4" max="4" width="16.14"/>
     <col customWidth="1" min="5" max="5" width="17.14"/>
     <col customWidth="1" min="6" max="6" width="12.57"/>
@@ -1402,33 +1159,33 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" ht="57.0" customHeight="1">
+    <row r="6" ht="59.25" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>1.0</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="1"/>
@@ -1448,26 +1205,34 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" ht="28.5" customHeight="1">
+    <row r="7" ht="59.25" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>17</v>
+      <c r="C7" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="E7" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1486,26 +1251,34 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" ht="43.5" customHeight="1">
+    <row r="8" ht="59.25" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15">
-        <v>3.0</v>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
       </c>
-      <c r="G8" s="15" t="s">
-        <v>23</v>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>24</v>
+      <c r="D8" s="8" t="s">
+        <v>28</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>25</v>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>26</v>
+      <c r="F8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1524,34 +1297,34 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" ht="42.75" customHeight="1">
+    <row r="9" ht="59.25" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="8" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
+      <c r="C9" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>29</v>
+      <c r="D9" s="8" t="s">
+        <v>35</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>30</v>
+      <c r="E9" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>1.0</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>31</v>
+      <c r="G9" s="8" t="s">
+        <v>37</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>32</v>
+      <c r="H9" s="8" t="s">
+        <v>38</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>33</v>
+      <c r="I9" s="8" t="s">
+        <v>39</v>
       </c>
-      <c r="J9" s="10" t="s">
-        <v>34</v>
+      <c r="J9" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1570,26 +1343,34 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" ht="42.75" customHeight="1">
+    <row r="10" ht="59.25" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12">
-        <v>2.0</v>
+      <c r="B10" s="8" t="s">
+        <v>41</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>35</v>
+      <c r="C10" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>36</v>
+      <c r="D10" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>37</v>
+      <c r="E10" s="8" t="s">
+        <v>43</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>38</v>
+      <c r="F10" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1608,26 +1389,34 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" ht="43.5" customHeight="1">
+    <row r="11" ht="59.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15">
-        <v>3.0</v>
+      <c r="B11" s="8" t="s">
+        <v>48</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>39</v>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>40</v>
+      <c r="D11" s="8" t="s">
+        <v>49</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>41</v>
+      <c r="E11" s="8" t="s">
+        <v>50</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>42</v>
+      <c r="F11" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1646,34 +1435,34 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" ht="57.0" customHeight="1">
+    <row r="12" ht="59.25" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>44</v>
+      <c r="D12" s="8" t="s">
+        <v>56</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>45</v>
+      <c r="E12" s="8" t="s">
+        <v>57</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>1.0</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>46</v>
+      <c r="G12" s="8" t="s">
+        <v>58</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>47</v>
+      <c r="H12" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>48</v>
+      <c r="I12" s="8" t="s">
+        <v>60</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>49</v>
+      <c r="J12" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1692,26 +1481,34 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" ht="28.5" customHeight="1">
+    <row r="13" ht="59.25" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12">
-        <v>2.0</v>
+      <c r="B13" s="8" t="s">
+        <v>62</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>50</v>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>51</v>
+      <c r="D13" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>52</v>
+      <c r="E13" s="8" t="s">
+        <v>64</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>53</v>
+      <c r="F13" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1730,26 +1527,34 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" ht="29.25" customHeight="1">
+    <row r="14" ht="59.25" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15">
-        <v>3.0</v>
+      <c r="B14" s="8" t="s">
+        <v>69</v>
       </c>
-      <c r="G14" s="15" t="s">
-        <v>54</v>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>55</v>
+      <c r="D14" s="8" t="s">
+        <v>70</v>
       </c>
-      <c r="I14" s="15" t="s">
-        <v>56</v>
+      <c r="E14" s="8" t="s">
+        <v>71</v>
       </c>
-      <c r="J14" s="16" t="s">
-        <v>57</v>
+      <c r="F14" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1768,34 +1573,34 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" ht="57.0" customHeight="1">
+    <row r="15" ht="59.25" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="8" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>28</v>
+      <c r="C15" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>59</v>
+      <c r="D15" s="8" t="s">
+        <v>77</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>60</v>
+      <c r="E15" s="8" t="s">
+        <v>78</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>1.0</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>61</v>
+      <c r="G15" s="8" t="s">
+        <v>79</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>62</v>
+      <c r="H15" s="8" t="s">
+        <v>80</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>63</v>
+      <c r="I15" s="8" t="s">
+        <v>81</v>
       </c>
-      <c r="J15" s="10" t="s">
-        <v>64</v>
+      <c r="J15" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1814,26 +1619,34 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" ht="43.5" customHeight="1">
+    <row r="16" ht="59.25" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15">
-        <v>2.0</v>
+      <c r="B16" s="8" t="s">
+        <v>83</v>
       </c>
-      <c r="G16" s="15" t="s">
-        <v>65</v>
+      <c r="C16" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H16" s="15" t="s">
-        <v>66</v>
+      <c r="D16" s="8" t="s">
+        <v>84</v>
       </c>
-      <c r="I16" s="15" t="s">
-        <v>67</v>
+      <c r="E16" s="8" t="s">
+        <v>85</v>
       </c>
-      <c r="J16" s="16" t="s">
-        <v>68</v>
+      <c r="F16" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1852,34 +1665,34 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" ht="42.75" customHeight="1">
+    <row r="17" ht="59.25" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="8" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>70</v>
+      <c r="C17" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>71</v>
+      <c r="D17" s="8" t="s">
+        <v>91</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>72</v>
+      <c r="E17" s="8" t="s">
+        <v>92</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>1.0</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>73</v>
+      <c r="G17" s="8" t="s">
+        <v>93</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>74</v>
+      <c r="H17" s="8" t="s">
+        <v>94</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>75</v>
+      <c r="I17" s="8" t="s">
+        <v>95</v>
       </c>
-      <c r="J17" s="10" t="s">
-        <v>76</v>
+      <c r="J17" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1898,26 +1711,34 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" ht="43.5" customHeight="1">
+    <row r="18" ht="59.25" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15">
-        <v>2.0</v>
+      <c r="B18" s="8" t="s">
+        <v>97</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>77</v>
+      <c r="C18" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>78</v>
+      <c r="D18" s="8" t="s">
+        <v>98</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="E18" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J18" s="16" t="s">
-        <v>80</v>
+      <c r="H18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1936,34 +1757,34 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" ht="72.0" customHeight="1">
+    <row r="19" ht="59.25" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="8" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>82</v>
+      <c r="D19" s="8" t="s">
+        <v>104</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>83</v>
+      <c r="E19" s="8" t="s">
+        <v>105</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>1.0</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>84</v>
+      <c r="G19" s="8" t="s">
+        <v>106</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>85</v>
+      <c r="H19" s="8" t="s">
+        <v>107</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>86</v>
+      <c r="I19" s="8" t="s">
+        <v>108</v>
       </c>
-      <c r="J19" s="10" t="s">
-        <v>87</v>
+      <c r="J19" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1982,26 +1803,34 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" ht="29.25" customHeight="1">
+    <row r="20" ht="59.25" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15">
-        <v>2.0</v>
+      <c r="B20" s="8" t="s">
+        <v>110</v>
       </c>
-      <c r="G20" s="15" t="s">
-        <v>88</v>
+      <c r="C20" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="H20" s="15" t="s">
-        <v>89</v>
+      <c r="D20" s="8" t="s">
+        <v>111</v>
       </c>
-      <c r="I20" s="15" t="s">
-        <v>90</v>
+      <c r="E20" s="8" t="s">
+        <v>112</v>
       </c>
-      <c r="J20" s="16" t="s">
-        <v>22</v>
+      <c r="F20" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2020,34 +1849,34 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" ht="57.75" customHeight="1">
+    <row r="21" ht="59.25" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="17" t="s">
-        <v>91</v>
+      <c r="B21" s="8" t="s">
+        <v>117</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>28</v>
+      <c r="C21" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>92</v>
+      <c r="D21" s="8" t="s">
+        <v>118</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>93</v>
+      <c r="E21" s="8" t="s">
+        <v>119</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="8">
         <v>1.0</v>
       </c>
-      <c r="G21" s="18" t="s">
-        <v>94</v>
+      <c r="G21" s="8" t="s">
+        <v>120</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>95</v>
+      <c r="H21" s="8" t="s">
+        <v>121</v>
       </c>
-      <c r="I21" s="18" t="s">
-        <v>96</v>
+      <c r="I21" s="8" t="s">
+        <v>122</v>
       </c>
-      <c r="J21" s="19" t="s">
-        <v>97</v>
+      <c r="J21" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -2066,34 +1895,34 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" ht="72.0" customHeight="1">
+    <row r="22" ht="59.25" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="17" t="s">
-        <v>98</v>
+      <c r="B22" s="8" t="s">
+        <v>124</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>99</v>
+      <c r="D22" s="8" t="s">
+        <v>125</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>100</v>
+      <c r="E22" s="8" t="s">
+        <v>126</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="8">
         <v>1.0</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>101</v>
+      <c r="G22" s="8" t="s">
+        <v>127</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>85</v>
+      <c r="H22" s="8" t="s">
+        <v>128</v>
       </c>
-      <c r="I22" s="18" t="s">
-        <v>102</v>
+      <c r="I22" s="8" t="s">
+        <v>129</v>
       </c>
-      <c r="J22" s="19" t="s">
-        <v>103</v>
+      <c r="J22" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2112,34 +1941,34 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" ht="43.5" customHeight="1">
+    <row r="23" ht="59.25" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="17" t="s">
-        <v>104</v>
+      <c r="B23" s="8" t="s">
+        <v>131</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>105</v>
+      <c r="D23" s="8" t="s">
+        <v>132</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>106</v>
+      <c r="E23" s="8" t="s">
+        <v>133</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="8">
         <v>1.0</v>
       </c>
-      <c r="G23" s="18" t="s">
-        <v>107</v>
+      <c r="G23" s="8" t="s">
+        <v>134</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>108</v>
+      <c r="H23" s="8" t="s">
+        <v>135</v>
       </c>
-      <c r="I23" s="18" t="s">
-        <v>109</v>
+      <c r="I23" s="8" t="s">
+        <v>136</v>
       </c>
-      <c r="J23" s="19" t="s">
-        <v>110</v>
+      <c r="J23" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2158,34 +1987,34 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" ht="57.75" customHeight="1">
+    <row r="24" ht="59.25" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="17" t="s">
-        <v>111</v>
+      <c r="B24" s="8" t="s">
+        <v>138</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>28</v>
+      <c r="C24" s="8" t="s">
+        <v>139</v>
       </c>
-      <c r="D24" s="18" t="s">
-        <v>112</v>
+      <c r="D24" s="8" t="s">
+        <v>140</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>113</v>
+      <c r="E24" s="8" t="s">
+        <v>141</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="8">
         <v>1.0</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>114</v>
+      <c r="G24" s="8" t="s">
+        <v>142</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>115</v>
+      <c r="H24" s="8" t="s">
+        <v>143</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>116</v>
+      <c r="I24" s="8" t="s">
+        <v>144</v>
       </c>
-      <c r="J24" s="19" t="s">
-        <v>117</v>
+      <c r="J24" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2204,34 +2033,34 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" ht="72.0" customHeight="1">
+    <row r="25" ht="59.25" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="17" t="s">
-        <v>118</v>
+      <c r="B25" s="8" t="s">
+        <v>146</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>119</v>
+      <c r="D25" s="8" t="s">
+        <v>147</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>120</v>
+      <c r="E25" s="8" t="s">
+        <v>148</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="8">
         <v>1.0</v>
       </c>
-      <c r="G25" s="18" t="s">
-        <v>121</v>
+      <c r="G25" s="8" t="s">
+        <v>149</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>122</v>
+      <c r="H25" s="8" t="s">
+        <v>150</v>
       </c>
-      <c r="I25" s="18" t="s">
-        <v>123</v>
+      <c r="I25" s="8" t="s">
+        <v>151</v>
       </c>
-      <c r="J25" s="19" t="s">
-        <v>124</v>
+      <c r="J25" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2250,34 +2079,34 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" ht="57.75" customHeight="1">
+    <row r="26" ht="59.25" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="17" t="s">
-        <v>125</v>
+      <c r="B26" s="8" t="s">
+        <v>153</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>28</v>
+      <c r="C26" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>126</v>
+      <c r="D26" s="8" t="s">
+        <v>154</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>127</v>
+      <c r="E26" s="8" t="s">
+        <v>155</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="8">
         <v>1.0</v>
       </c>
-      <c r="G26" s="18" t="s">
-        <v>128</v>
+      <c r="G26" s="8" t="s">
+        <v>156</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>129</v>
+      <c r="H26" s="8" t="s">
+        <v>157</v>
       </c>
-      <c r="I26" s="18" t="s">
-        <v>130</v>
+      <c r="I26" s="8" t="s">
+        <v>158</v>
       </c>
-      <c r="J26" s="19" t="s">
-        <v>131</v>
+      <c r="J26" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2296,34 +2125,34 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" ht="57.75" customHeight="1">
+    <row r="27" ht="59.25" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="17" t="s">
-        <v>132</v>
+      <c r="B27" s="8" t="s">
+        <v>160</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>119</v>
+      <c r="D27" s="8" t="s">
+        <v>161</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>133</v>
+      <c r="E27" s="8" t="s">
+        <v>162</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="8">
         <v>1.0</v>
       </c>
-      <c r="G27" s="18" t="s">
-        <v>134</v>
+      <c r="G27" s="8" t="s">
+        <v>163</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>135</v>
+      <c r="H27" s="8" t="s">
+        <v>164</v>
       </c>
-      <c r="I27" s="18" t="s">
-        <v>136</v>
+      <c r="I27" s="8" t="s">
+        <v>165</v>
       </c>
-      <c r="J27" s="19" t="s">
-        <v>137</v>
+      <c r="J27" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2342,34 +2171,34 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" ht="57.75" customHeight="1">
+    <row r="28" ht="59.25" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="17" t="s">
-        <v>138</v>
+      <c r="B28" s="8" t="s">
+        <v>167</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>70</v>
+      <c r="C28" s="8" t="s">
+        <v>13</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>139</v>
+      <c r="D28" s="8" t="s">
+        <v>168</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>140</v>
+      <c r="E28" s="8" t="s">
+        <v>169</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="8">
         <v>1.0</v>
       </c>
-      <c r="G28" s="18" t="s">
-        <v>141</v>
+      <c r="G28" s="8" t="s">
+        <v>170</v>
       </c>
-      <c r="H28" s="18" t="s">
-        <v>142</v>
+      <c r="H28" s="8" t="s">
+        <v>171</v>
       </c>
-      <c r="I28" s="18" t="s">
-        <v>143</v>
+      <c r="I28" s="8" t="s">
+        <v>172</v>
       </c>
-      <c r="J28" s="19" t="s">
-        <v>144</v>
+      <c r="J28" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -2388,17 +2217,35 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" ht="59.25" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="B29" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -28791,818 +28638,6 @@
       <c r="X971" s="1"/>
       <c r="Y971" s="1"/>
       <c r="Z971" s="1"/>
-    </row>
-    <row r="972" ht="14.25" customHeight="1">
-      <c r="A972" s="1"/>
-      <c r="B972" s="1"/>
-      <c r="C972" s="1"/>
-      <c r="D972" s="1"/>
-      <c r="E972" s="1"/>
-      <c r="F972" s="1"/>
-      <c r="G972" s="1"/>
-      <c r="H972" s="1"/>
-      <c r="I972" s="1"/>
-      <c r="J972" s="1"/>
-      <c r="K972" s="1"/>
-      <c r="L972" s="1"/>
-      <c r="M972" s="1"/>
-      <c r="N972" s="1"/>
-      <c r="O972" s="1"/>
-      <c r="P972" s="1"/>
-      <c r="Q972" s="1"/>
-      <c r="R972" s="1"/>
-      <c r="S972" s="1"/>
-      <c r="T972" s="1"/>
-      <c r="U972" s="1"/>
-      <c r="V972" s="1"/>
-      <c r="W972" s="1"/>
-      <c r="X972" s="1"/>
-      <c r="Y972" s="1"/>
-      <c r="Z972" s="1"/>
-    </row>
-    <row r="973" ht="14.25" customHeight="1">
-      <c r="A973" s="1"/>
-      <c r="B973" s="1"/>
-      <c r="C973" s="1"/>
-      <c r="D973" s="1"/>
-      <c r="E973" s="1"/>
-      <c r="F973" s="1"/>
-      <c r="G973" s="1"/>
-      <c r="H973" s="1"/>
-      <c r="I973" s="1"/>
-      <c r="J973" s="1"/>
-      <c r="K973" s="1"/>
-      <c r="L973" s="1"/>
-      <c r="M973" s="1"/>
-      <c r="N973" s="1"/>
-      <c r="O973" s="1"/>
-      <c r="P973" s="1"/>
-      <c r="Q973" s="1"/>
-      <c r="R973" s="1"/>
-      <c r="S973" s="1"/>
-      <c r="T973" s="1"/>
-      <c r="U973" s="1"/>
-      <c r="V973" s="1"/>
-      <c r="W973" s="1"/>
-      <c r="X973" s="1"/>
-      <c r="Y973" s="1"/>
-      <c r="Z973" s="1"/>
-    </row>
-    <row r="974" ht="14.25" customHeight="1">
-      <c r="A974" s="1"/>
-      <c r="B974" s="1"/>
-      <c r="C974" s="1"/>
-      <c r="D974" s="1"/>
-      <c r="E974" s="1"/>
-      <c r="F974" s="1"/>
-      <c r="G974" s="1"/>
-      <c r="H974" s="1"/>
-      <c r="I974" s="1"/>
-      <c r="J974" s="1"/>
-      <c r="K974" s="1"/>
-      <c r="L974" s="1"/>
-      <c r="M974" s="1"/>
-      <c r="N974" s="1"/>
-      <c r="O974" s="1"/>
-      <c r="P974" s="1"/>
-      <c r="Q974" s="1"/>
-      <c r="R974" s="1"/>
-      <c r="S974" s="1"/>
-      <c r="T974" s="1"/>
-      <c r="U974" s="1"/>
-      <c r="V974" s="1"/>
-      <c r="W974" s="1"/>
-      <c r="X974" s="1"/>
-      <c r="Y974" s="1"/>
-      <c r="Z974" s="1"/>
-    </row>
-    <row r="975" ht="14.25" customHeight="1">
-      <c r="A975" s="1"/>
-      <c r="B975" s="1"/>
-      <c r="C975" s="1"/>
-      <c r="D975" s="1"/>
-      <c r="E975" s="1"/>
-      <c r="F975" s="1"/>
-      <c r="G975" s="1"/>
-      <c r="H975" s="1"/>
-      <c r="I975" s="1"/>
-      <c r="J975" s="1"/>
-      <c r="K975" s="1"/>
-      <c r="L975" s="1"/>
-      <c r="M975" s="1"/>
-      <c r="N975" s="1"/>
-      <c r="O975" s="1"/>
-      <c r="P975" s="1"/>
-      <c r="Q975" s="1"/>
-      <c r="R975" s="1"/>
-      <c r="S975" s="1"/>
-      <c r="T975" s="1"/>
-      <c r="U975" s="1"/>
-      <c r="V975" s="1"/>
-      <c r="W975" s="1"/>
-      <c r="X975" s="1"/>
-      <c r="Y975" s="1"/>
-      <c r="Z975" s="1"/>
-    </row>
-    <row r="976" ht="14.25" customHeight="1">
-      <c r="A976" s="1"/>
-      <c r="B976" s="1"/>
-      <c r="C976" s="1"/>
-      <c r="D976" s="1"/>
-      <c r="E976" s="1"/>
-      <c r="F976" s="1"/>
-      <c r="G976" s="1"/>
-      <c r="H976" s="1"/>
-      <c r="I976" s="1"/>
-      <c r="J976" s="1"/>
-      <c r="K976" s="1"/>
-      <c r="L976" s="1"/>
-      <c r="M976" s="1"/>
-      <c r="N976" s="1"/>
-      <c r="O976" s="1"/>
-      <c r="P976" s="1"/>
-      <c r="Q976" s="1"/>
-      <c r="R976" s="1"/>
-      <c r="S976" s="1"/>
-      <c r="T976" s="1"/>
-      <c r="U976" s="1"/>
-      <c r="V976" s="1"/>
-      <c r="W976" s="1"/>
-      <c r="X976" s="1"/>
-      <c r="Y976" s="1"/>
-      <c r="Z976" s="1"/>
-    </row>
-    <row r="977" ht="14.25" customHeight="1">
-      <c r="A977" s="1"/>
-      <c r="B977" s="1"/>
-      <c r="C977" s="1"/>
-      <c r="D977" s="1"/>
-      <c r="E977" s="1"/>
-      <c r="F977" s="1"/>
-      <c r="G977" s="1"/>
-      <c r="H977" s="1"/>
-      <c r="I977" s="1"/>
-      <c r="J977" s="1"/>
-      <c r="K977" s="1"/>
-      <c r="L977" s="1"/>
-      <c r="M977" s="1"/>
-      <c r="N977" s="1"/>
-      <c r="O977" s="1"/>
-      <c r="P977" s="1"/>
-      <c r="Q977" s="1"/>
-      <c r="R977" s="1"/>
-      <c r="S977" s="1"/>
-      <c r="T977" s="1"/>
-      <c r="U977" s="1"/>
-      <c r="V977" s="1"/>
-      <c r="W977" s="1"/>
-      <c r="X977" s="1"/>
-      <c r="Y977" s="1"/>
-      <c r="Z977" s="1"/>
-    </row>
-    <row r="978" ht="14.25" customHeight="1">
-      <c r="A978" s="1"/>
-      <c r="B978" s="1"/>
-      <c r="C978" s="1"/>
-      <c r="D978" s="1"/>
-      <c r="E978" s="1"/>
-      <c r="F978" s="1"/>
-      <c r="G978" s="1"/>
-      <c r="H978" s="1"/>
-      <c r="I978" s="1"/>
-      <c r="J978" s="1"/>
-      <c r="K978" s="1"/>
-      <c r="L978" s="1"/>
-      <c r="M978" s="1"/>
-      <c r="N978" s="1"/>
-      <c r="O978" s="1"/>
-      <c r="P978" s="1"/>
-      <c r="Q978" s="1"/>
-      <c r="R978" s="1"/>
-      <c r="S978" s="1"/>
-      <c r="T978" s="1"/>
-      <c r="U978" s="1"/>
-      <c r="V978" s="1"/>
-      <c r="W978" s="1"/>
-      <c r="X978" s="1"/>
-      <c r="Y978" s="1"/>
-      <c r="Z978" s="1"/>
-    </row>
-    <row r="979" ht="14.25" customHeight="1">
-      <c r="A979" s="1"/>
-      <c r="B979" s="1"/>
-      <c r="C979" s="1"/>
-      <c r="D979" s="1"/>
-      <c r="E979" s="1"/>
-      <c r="F979" s="1"/>
-      <c r="G979" s="1"/>
-      <c r="H979" s="1"/>
-      <c r="I979" s="1"/>
-      <c r="J979" s="1"/>
-      <c r="K979" s="1"/>
-      <c r="L979" s="1"/>
-      <c r="M979" s="1"/>
-      <c r="N979" s="1"/>
-      <c r="O979" s="1"/>
-      <c r="P979" s="1"/>
-      <c r="Q979" s="1"/>
-      <c r="R979" s="1"/>
-      <c r="S979" s="1"/>
-      <c r="T979" s="1"/>
-      <c r="U979" s="1"/>
-      <c r="V979" s="1"/>
-      <c r="W979" s="1"/>
-      <c r="X979" s="1"/>
-      <c r="Y979" s="1"/>
-      <c r="Z979" s="1"/>
-    </row>
-    <row r="980" ht="14.25" customHeight="1">
-      <c r="A980" s="1"/>
-      <c r="B980" s="1"/>
-      <c r="C980" s="1"/>
-      <c r="D980" s="1"/>
-      <c r="E980" s="1"/>
-      <c r="F980" s="1"/>
-      <c r="G980" s="1"/>
-      <c r="H980" s="1"/>
-      <c r="I980" s="1"/>
-      <c r="J980" s="1"/>
-      <c r="K980" s="1"/>
-      <c r="L980" s="1"/>
-      <c r="M980" s="1"/>
-      <c r="N980" s="1"/>
-      <c r="O980" s="1"/>
-      <c r="P980" s="1"/>
-      <c r="Q980" s="1"/>
-      <c r="R980" s="1"/>
-      <c r="S980" s="1"/>
-      <c r="T980" s="1"/>
-      <c r="U980" s="1"/>
-      <c r="V980" s="1"/>
-      <c r="W980" s="1"/>
-      <c r="X980" s="1"/>
-      <c r="Y980" s="1"/>
-      <c r="Z980" s="1"/>
-    </row>
-    <row r="981" ht="14.25" customHeight="1">
-      <c r="A981" s="1"/>
-      <c r="B981" s="1"/>
-      <c r="C981" s="1"/>
-      <c r="D981" s="1"/>
-      <c r="E981" s="1"/>
-      <c r="F981" s="1"/>
-      <c r="G981" s="1"/>
-      <c r="H981" s="1"/>
-      <c r="I981" s="1"/>
-      <c r="J981" s="1"/>
-      <c r="K981" s="1"/>
-      <c r="L981" s="1"/>
-      <c r="M981" s="1"/>
-      <c r="N981" s="1"/>
-      <c r="O981" s="1"/>
-      <c r="P981" s="1"/>
-      <c r="Q981" s="1"/>
-      <c r="R981" s="1"/>
-      <c r="S981" s="1"/>
-      <c r="T981" s="1"/>
-      <c r="U981" s="1"/>
-      <c r="V981" s="1"/>
-      <c r="W981" s="1"/>
-      <c r="X981" s="1"/>
-      <c r="Y981" s="1"/>
-      <c r="Z981" s="1"/>
-    </row>
-    <row r="982" ht="14.25" customHeight="1">
-      <c r="A982" s="1"/>
-      <c r="B982" s="1"/>
-      <c r="C982" s="1"/>
-      <c r="D982" s="1"/>
-      <c r="E982" s="1"/>
-      <c r="F982" s="1"/>
-      <c r="G982" s="1"/>
-      <c r="H982" s="1"/>
-      <c r="I982" s="1"/>
-      <c r="J982" s="1"/>
-      <c r="K982" s="1"/>
-      <c r="L982" s="1"/>
-      <c r="M982" s="1"/>
-      <c r="N982" s="1"/>
-      <c r="O982" s="1"/>
-      <c r="P982" s="1"/>
-      <c r="Q982" s="1"/>
-      <c r="R982" s="1"/>
-      <c r="S982" s="1"/>
-      <c r="T982" s="1"/>
-      <c r="U982" s="1"/>
-      <c r="V982" s="1"/>
-      <c r="W982" s="1"/>
-      <c r="X982" s="1"/>
-      <c r="Y982" s="1"/>
-      <c r="Z982" s="1"/>
-    </row>
-    <row r="983" ht="14.25" customHeight="1">
-      <c r="A983" s="1"/>
-      <c r="B983" s="1"/>
-      <c r="C983" s="1"/>
-      <c r="D983" s="1"/>
-      <c r="E983" s="1"/>
-      <c r="F983" s="1"/>
-      <c r="G983" s="1"/>
-      <c r="H983" s="1"/>
-      <c r="I983" s="1"/>
-      <c r="J983" s="1"/>
-      <c r="K983" s="1"/>
-      <c r="L983" s="1"/>
-      <c r="M983" s="1"/>
-      <c r="N983" s="1"/>
-      <c r="O983" s="1"/>
-      <c r="P983" s="1"/>
-      <c r="Q983" s="1"/>
-      <c r="R983" s="1"/>
-      <c r="S983" s="1"/>
-      <c r="T983" s="1"/>
-      <c r="U983" s="1"/>
-      <c r="V983" s="1"/>
-      <c r="W983" s="1"/>
-      <c r="X983" s="1"/>
-      <c r="Y983" s="1"/>
-      <c r="Z983" s="1"/>
-    </row>
-    <row r="984" ht="14.25" customHeight="1">
-      <c r="A984" s="1"/>
-      <c r="B984" s="1"/>
-      <c r="C984" s="1"/>
-      <c r="D984" s="1"/>
-      <c r="E984" s="1"/>
-      <c r="F984" s="1"/>
-      <c r="G984" s="1"/>
-      <c r="H984" s="1"/>
-      <c r="I984" s="1"/>
-      <c r="J984" s="1"/>
-      <c r="K984" s="1"/>
-      <c r="L984" s="1"/>
-      <c r="M984" s="1"/>
-      <c r="N984" s="1"/>
-      <c r="O984" s="1"/>
-      <c r="P984" s="1"/>
-      <c r="Q984" s="1"/>
-      <c r="R984" s="1"/>
-      <c r="S984" s="1"/>
-      <c r="T984" s="1"/>
-      <c r="U984" s="1"/>
-      <c r="V984" s="1"/>
-      <c r="W984" s="1"/>
-      <c r="X984" s="1"/>
-      <c r="Y984" s="1"/>
-      <c r="Z984" s="1"/>
-    </row>
-    <row r="985" ht="14.25" customHeight="1">
-      <c r="A985" s="1"/>
-      <c r="B985" s="1"/>
-      <c r="C985" s="1"/>
-      <c r="D985" s="1"/>
-      <c r="E985" s="1"/>
-      <c r="F985" s="1"/>
-      <c r="G985" s="1"/>
-      <c r="H985" s="1"/>
-      <c r="I985" s="1"/>
-      <c r="J985" s="1"/>
-      <c r="K985" s="1"/>
-      <c r="L985" s="1"/>
-      <c r="M985" s="1"/>
-      <c r="N985" s="1"/>
-      <c r="O985" s="1"/>
-      <c r="P985" s="1"/>
-      <c r="Q985" s="1"/>
-      <c r="R985" s="1"/>
-      <c r="S985" s="1"/>
-      <c r="T985" s="1"/>
-      <c r="U985" s="1"/>
-      <c r="V985" s="1"/>
-      <c r="W985" s="1"/>
-      <c r="X985" s="1"/>
-      <c r="Y985" s="1"/>
-      <c r="Z985" s="1"/>
-    </row>
-    <row r="986" ht="14.25" customHeight="1">
-      <c r="A986" s="1"/>
-      <c r="B986" s="1"/>
-      <c r="C986" s="1"/>
-      <c r="D986" s="1"/>
-      <c r="E986" s="1"/>
-      <c r="F986" s="1"/>
-      <c r="G986" s="1"/>
-      <c r="H986" s="1"/>
-      <c r="I986" s="1"/>
-      <c r="J986" s="1"/>
-      <c r="K986" s="1"/>
-      <c r="L986" s="1"/>
-      <c r="M986" s="1"/>
-      <c r="N986" s="1"/>
-      <c r="O986" s="1"/>
-      <c r="P986" s="1"/>
-      <c r="Q986" s="1"/>
-      <c r="R986" s="1"/>
-      <c r="S986" s="1"/>
-      <c r="T986" s="1"/>
-      <c r="U986" s="1"/>
-      <c r="V986" s="1"/>
-      <c r="W986" s="1"/>
-      <c r="X986" s="1"/>
-      <c r="Y986" s="1"/>
-      <c r="Z986" s="1"/>
-    </row>
-    <row r="987" ht="14.25" customHeight="1">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="C987" s="1"/>
-      <c r="D987" s="1"/>
-      <c r="E987" s="1"/>
-      <c r="F987" s="1"/>
-      <c r="G987" s="1"/>
-      <c r="H987" s="1"/>
-      <c r="I987" s="1"/>
-      <c r="J987" s="1"/>
-      <c r="K987" s="1"/>
-      <c r="L987" s="1"/>
-      <c r="M987" s="1"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="1"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-      <c r="T987" s="1"/>
-      <c r="U987" s="1"/>
-      <c r="V987" s="1"/>
-      <c r="W987" s="1"/>
-      <c r="X987" s="1"/>
-      <c r="Y987" s="1"/>
-      <c r="Z987" s="1"/>
-    </row>
-    <row r="988" ht="14.25" customHeight="1">
-      <c r="A988" s="1"/>
-      <c r="B988" s="1"/>
-      <c r="C988" s="1"/>
-      <c r="D988" s="1"/>
-      <c r="E988" s="1"/>
-      <c r="F988" s="1"/>
-      <c r="G988" s="1"/>
-      <c r="H988" s="1"/>
-      <c r="I988" s="1"/>
-      <c r="J988" s="1"/>
-      <c r="K988" s="1"/>
-      <c r="L988" s="1"/>
-      <c r="M988" s="1"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="1"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-      <c r="T988" s="1"/>
-      <c r="U988" s="1"/>
-      <c r="V988" s="1"/>
-      <c r="W988" s="1"/>
-      <c r="X988" s="1"/>
-      <c r="Y988" s="1"/>
-      <c r="Z988" s="1"/>
-    </row>
-    <row r="989" ht="14.25" customHeight="1">
-      <c r="A989" s="1"/>
-      <c r="B989" s="1"/>
-      <c r="C989" s="1"/>
-      <c r="D989" s="1"/>
-      <c r="E989" s="1"/>
-      <c r="F989" s="1"/>
-      <c r="G989" s="1"/>
-      <c r="H989" s="1"/>
-      <c r="I989" s="1"/>
-      <c r="J989" s="1"/>
-      <c r="K989" s="1"/>
-      <c r="L989" s="1"/>
-      <c r="M989" s="1"/>
-      <c r="N989" s="1"/>
-      <c r="O989" s="1"/>
-      <c r="P989" s="1"/>
-      <c r="Q989" s="1"/>
-      <c r="R989" s="1"/>
-      <c r="S989" s="1"/>
-      <c r="T989" s="1"/>
-      <c r="U989" s="1"/>
-      <c r="V989" s="1"/>
-      <c r="W989" s="1"/>
-      <c r="X989" s="1"/>
-      <c r="Y989" s="1"/>
-      <c r="Z989" s="1"/>
-    </row>
-    <row r="990" ht="14.25" customHeight="1">
-      <c r="A990" s="1"/>
-      <c r="B990" s="1"/>
-      <c r="C990" s="1"/>
-      <c r="D990" s="1"/>
-      <c r="E990" s="1"/>
-      <c r="F990" s="1"/>
-      <c r="G990" s="1"/>
-      <c r="H990" s="1"/>
-      <c r="I990" s="1"/>
-      <c r="J990" s="1"/>
-      <c r="K990" s="1"/>
-      <c r="L990" s="1"/>
-      <c r="M990" s="1"/>
-      <c r="N990" s="1"/>
-      <c r="O990" s="1"/>
-      <c r="P990" s="1"/>
-      <c r="Q990" s="1"/>
-      <c r="R990" s="1"/>
-      <c r="S990" s="1"/>
-      <c r="T990" s="1"/>
-      <c r="U990" s="1"/>
-      <c r="V990" s="1"/>
-      <c r="W990" s="1"/>
-      <c r="X990" s="1"/>
-      <c r="Y990" s="1"/>
-      <c r="Z990" s="1"/>
-    </row>
-    <row r="991" ht="14.25" customHeight="1">
-      <c r="A991" s="1"/>
-      <c r="B991" s="1"/>
-      <c r="C991" s="1"/>
-      <c r="D991" s="1"/>
-      <c r="E991" s="1"/>
-      <c r="F991" s="1"/>
-      <c r="G991" s="1"/>
-      <c r="H991" s="1"/>
-      <c r="I991" s="1"/>
-      <c r="J991" s="1"/>
-      <c r="K991" s="1"/>
-      <c r="L991" s="1"/>
-      <c r="M991" s="1"/>
-      <c r="N991" s="1"/>
-      <c r="O991" s="1"/>
-      <c r="P991" s="1"/>
-      <c r="Q991" s="1"/>
-      <c r="R991" s="1"/>
-      <c r="S991" s="1"/>
-      <c r="T991" s="1"/>
-      <c r="U991" s="1"/>
-      <c r="V991" s="1"/>
-      <c r="W991" s="1"/>
-      <c r="X991" s="1"/>
-      <c r="Y991" s="1"/>
-      <c r="Z991" s="1"/>
-    </row>
-    <row r="992" ht="14.25" customHeight="1">
-      <c r="A992" s="1"/>
-      <c r="B992" s="1"/>
-      <c r="C992" s="1"/>
-      <c r="D992" s="1"/>
-      <c r="E992" s="1"/>
-      <c r="F992" s="1"/>
-      <c r="G992" s="1"/>
-      <c r="H992" s="1"/>
-      <c r="I992" s="1"/>
-      <c r="J992" s="1"/>
-      <c r="K992" s="1"/>
-      <c r="L992" s="1"/>
-      <c r="M992" s="1"/>
-      <c r="N992" s="1"/>
-      <c r="O992" s="1"/>
-      <c r="P992" s="1"/>
-      <c r="Q992" s="1"/>
-      <c r="R992" s="1"/>
-      <c r="S992" s="1"/>
-      <c r="T992" s="1"/>
-      <c r="U992" s="1"/>
-      <c r="V992" s="1"/>
-      <c r="W992" s="1"/>
-      <c r="X992" s="1"/>
-      <c r="Y992" s="1"/>
-      <c r="Z992" s="1"/>
-    </row>
-    <row r="993" ht="14.25" customHeight="1">
-      <c r="A993" s="1"/>
-      <c r="B993" s="1"/>
-      <c r="C993" s="1"/>
-      <c r="D993" s="1"/>
-      <c r="E993" s="1"/>
-      <c r="F993" s="1"/>
-      <c r="G993" s="1"/>
-      <c r="H993" s="1"/>
-      <c r="I993" s="1"/>
-      <c r="J993" s="1"/>
-      <c r="K993" s="1"/>
-      <c r="L993" s="1"/>
-      <c r="M993" s="1"/>
-      <c r="N993" s="1"/>
-      <c r="O993" s="1"/>
-      <c r="P993" s="1"/>
-      <c r="Q993" s="1"/>
-      <c r="R993" s="1"/>
-      <c r="S993" s="1"/>
-      <c r="T993" s="1"/>
-      <c r="U993" s="1"/>
-      <c r="V993" s="1"/>
-      <c r="W993" s="1"/>
-      <c r="X993" s="1"/>
-      <c r="Y993" s="1"/>
-      <c r="Z993" s="1"/>
-    </row>
-    <row r="994" ht="14.25" customHeight="1">
-      <c r="A994" s="1"/>
-      <c r="B994" s="1"/>
-      <c r="C994" s="1"/>
-      <c r="D994" s="1"/>
-      <c r="E994" s="1"/>
-      <c r="F994" s="1"/>
-      <c r="G994" s="1"/>
-      <c r="H994" s="1"/>
-      <c r="I994" s="1"/>
-      <c r="J994" s="1"/>
-      <c r="K994" s="1"/>
-      <c r="L994" s="1"/>
-      <c r="M994" s="1"/>
-      <c r="N994" s="1"/>
-      <c r="O994" s="1"/>
-      <c r="P994" s="1"/>
-      <c r="Q994" s="1"/>
-      <c r="R994" s="1"/>
-      <c r="S994" s="1"/>
-      <c r="T994" s="1"/>
-      <c r="U994" s="1"/>
-      <c r="V994" s="1"/>
-      <c r="W994" s="1"/>
-      <c r="X994" s="1"/>
-      <c r="Y994" s="1"/>
-      <c r="Z994" s="1"/>
-    </row>
-    <row r="995" ht="14.25" customHeight="1">
-      <c r="A995" s="1"/>
-      <c r="B995" s="1"/>
-      <c r="C995" s="1"/>
-      <c r="D995" s="1"/>
-      <c r="E995" s="1"/>
-      <c r="F995" s="1"/>
-      <c r="G995" s="1"/>
-      <c r="H995" s="1"/>
-      <c r="I995" s="1"/>
-      <c r="J995" s="1"/>
-      <c r="K995" s="1"/>
-      <c r="L995" s="1"/>
-      <c r="M995" s="1"/>
-      <c r="N995" s="1"/>
-      <c r="O995" s="1"/>
-      <c r="P995" s="1"/>
-      <c r="Q995" s="1"/>
-      <c r="R995" s="1"/>
-      <c r="S995" s="1"/>
-      <c r="T995" s="1"/>
-      <c r="U995" s="1"/>
-      <c r="V995" s="1"/>
-      <c r="W995" s="1"/>
-      <c r="X995" s="1"/>
-      <c r="Y995" s="1"/>
-      <c r="Z995" s="1"/>
-    </row>
-    <row r="996" ht="14.25" customHeight="1">
-      <c r="A996" s="1"/>
-      <c r="B996" s="1"/>
-      <c r="C996" s="1"/>
-      <c r="D996" s="1"/>
-      <c r="E996" s="1"/>
-      <c r="F996" s="1"/>
-      <c r="G996" s="1"/>
-      <c r="H996" s="1"/>
-      <c r="I996" s="1"/>
-      <c r="J996" s="1"/>
-      <c r="K996" s="1"/>
-      <c r="L996" s="1"/>
-      <c r="M996" s="1"/>
-      <c r="N996" s="1"/>
-      <c r="O996" s="1"/>
-      <c r="P996" s="1"/>
-      <c r="Q996" s="1"/>
-      <c r="R996" s="1"/>
-      <c r="S996" s="1"/>
-      <c r="T996" s="1"/>
-      <c r="U996" s="1"/>
-      <c r="V996" s="1"/>
-      <c r="W996" s="1"/>
-      <c r="X996" s="1"/>
-      <c r="Y996" s="1"/>
-      <c r="Z996" s="1"/>
-    </row>
-    <row r="997" ht="14.25" customHeight="1">
-      <c r="A997" s="1"/>
-      <c r="B997" s="1"/>
-      <c r="C997" s="1"/>
-      <c r="D997" s="1"/>
-      <c r="E997" s="1"/>
-      <c r="F997" s="1"/>
-      <c r="G997" s="1"/>
-      <c r="H997" s="1"/>
-      <c r="I997" s="1"/>
-      <c r="J997" s="1"/>
-      <c r="K997" s="1"/>
-      <c r="L997" s="1"/>
-      <c r="M997" s="1"/>
-      <c r="N997" s="1"/>
-      <c r="O997" s="1"/>
-      <c r="P997" s="1"/>
-      <c r="Q997" s="1"/>
-      <c r="R997" s="1"/>
-      <c r="S997" s="1"/>
-      <c r="T997" s="1"/>
-      <c r="U997" s="1"/>
-      <c r="V997" s="1"/>
-      <c r="W997" s="1"/>
-      <c r="X997" s="1"/>
-      <c r="Y997" s="1"/>
-      <c r="Z997" s="1"/>
-    </row>
-    <row r="998" ht="14.25" customHeight="1">
-      <c r="A998" s="1"/>
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="1"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-    </row>
-    <row r="999" ht="14.25" customHeight="1">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="1"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="1"/>
-      <c r="G999" s="1"/>
-      <c r="H999" s="1"/>
-      <c r="I999" s="1"/>
-      <c r="J999" s="1"/>
-      <c r="K999" s="1"/>
-      <c r="L999" s="1"/>
-      <c r="M999" s="1"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-    </row>
-    <row r="1000" ht="14.25" customHeight="1">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="1"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="1"/>
-      <c r="K1000" s="1"/>
-      <c r="L1000" s="1"/>
-      <c r="M1000" s="1"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -29636,8 +28671,8 @@
   <sheetData>
     <row r="1" ht="30.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
-        <v>145</v>
+      <c r="B1" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -29667,7 +28702,7 @@
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -29724,11 +28759,11 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="21" t="s">
-        <v>147</v>
+      <c r="B4" s="10" t="s">
+        <v>183</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>148</v>
+      <c r="C4" s="10" t="s">
+        <v>184</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -29756,11 +28791,11 @@
     </row>
     <row r="5" ht="28.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>149</v>
+      <c r="C5" s="11" t="s">
+        <v>185</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -29788,11 +28823,11 @@
     </row>
     <row r="6" ht="129.0" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>150</v>
+      <c r="C6" s="11" t="s">
+        <v>186</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -29820,11 +28855,11 @@
     </row>
     <row r="7" ht="100.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>151</v>
+      <c r="C7" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -29852,11 +28887,11 @@
     </row>
     <row r="8" ht="42.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>152</v>
+      <c r="C8" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -29884,11 +28919,11 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>153</v>
+      <c r="C9" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -29916,11 +28951,11 @@
     </row>
     <row r="10" ht="42.75" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="22" t="s">
-        <v>154</v>
+      <c r="B10" s="11" t="s">
+        <v>190</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>155</v>
+      <c r="C10" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -29948,11 +28983,11 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>156</v>
+      <c r="C11" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -29980,11 +29015,11 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>157</v>
+      <c r="C12" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -30012,11 +29047,11 @@
     </row>
     <row r="13" ht="28.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>158</v>
+      <c r="C13" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -57684,1195 +56719,4 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="9" width="24.29"/>
-    <col customWidth="1" min="10" max="26" width="10.0"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="36.0" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-    </row>
-    <row r="2" ht="21.0" customHeight="1">
-      <c r="A2" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" ht="28.5" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" ht="57.0" customHeight="1">
-      <c r="A6" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" ht="57.0" customHeight="1">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" ht="42.75" customHeight="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="32">
-        <v>3.0</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-  </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>